<commit_message>
forgot to add column info
</commit_message>
<xml_diff>
--- a/Milestone_2/data/demographics.xlsx
+++ b/Milestone_2/data/demographics.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vikram/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vikram/Desktop/repos/CS348_project/Milestone_2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{17B19181-E07F-6A45-974D-A093E28EBE1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E78C31-ECC3-954F-90A5-6B5E61239288}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7680" yWindow="3220" windowWidth="27640" windowHeight="16940" xr2:uid="{86A1A427-D4BE-7D4F-9F97-547C545D3F98}"/>
+    <workbookView xWindow="7680" yWindow="3160" windowWidth="27640" windowHeight="16940" xr2:uid="{86A1A427-D4BE-7D4F-9F97-547C545D3F98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="175">
   <si>
     <t>Education</t>
   </si>
@@ -120,6 +120,444 @@
   </si>
   <si>
     <t>EMPLOYMENT</t>
+  </si>
+  <si>
+    <t>_id</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>Data Source</t>
+  </si>
+  <si>
+    <t>Characteristic</t>
+  </si>
+  <si>
+    <t>City of Toronto</t>
+  </si>
+  <si>
+    <t>Agincourt North</t>
+  </si>
+  <si>
+    <t>Agincourt South-Malvern West</t>
+  </si>
+  <si>
+    <t>Alderwood</t>
+  </si>
+  <si>
+    <t>Annex</t>
+  </si>
+  <si>
+    <t>Banbury-Don Mills</t>
+  </si>
+  <si>
+    <t>Bathurst Manor</t>
+  </si>
+  <si>
+    <t>Bay Street Corridor</t>
+  </si>
+  <si>
+    <t>Bayview Village</t>
+  </si>
+  <si>
+    <t>Bayview Woods-Steeles</t>
+  </si>
+  <si>
+    <t>Bedford Park-Nortown</t>
+  </si>
+  <si>
+    <t>Beechborough-Greenbrook</t>
+  </si>
+  <si>
+    <t>Bendale</t>
+  </si>
+  <si>
+    <t>Birchcliffe-Cliffside</t>
+  </si>
+  <si>
+    <t>Black Creek</t>
+  </si>
+  <si>
+    <t>Blake-Jones</t>
+  </si>
+  <si>
+    <t>Briar Hill-Belgravia</t>
+  </si>
+  <si>
+    <t>Bridle Path-Sunnybrook-York Mills</t>
+  </si>
+  <si>
+    <t>Broadview North</t>
+  </si>
+  <si>
+    <t>Brookhaven-Amesbury</t>
+  </si>
+  <si>
+    <t>Cabbagetown-South St. James Town</t>
+  </si>
+  <si>
+    <t>Caledonia-Fairbank</t>
+  </si>
+  <si>
+    <t>Casa Loma</t>
+  </si>
+  <si>
+    <t>Centennial Scarborough</t>
+  </si>
+  <si>
+    <t>Church-Yonge Corridor</t>
+  </si>
+  <si>
+    <t>Clairlea-Birchmount</t>
+  </si>
+  <si>
+    <t>Clanton Park</t>
+  </si>
+  <si>
+    <t>Cliffcrest</t>
+  </si>
+  <si>
+    <t>Corso Italia-Davenport</t>
+  </si>
+  <si>
+    <t>Danforth</t>
+  </si>
+  <si>
+    <t>Danforth East York</t>
+  </si>
+  <si>
+    <t>Don Valley Village</t>
+  </si>
+  <si>
+    <t>Dorset Park</t>
+  </si>
+  <si>
+    <t>Dovercourt-Wallace Emerson-Junction</t>
+  </si>
+  <si>
+    <t>Downsview-Roding-CFB</t>
+  </si>
+  <si>
+    <t>Dufferin Grove</t>
+  </si>
+  <si>
+    <t>East End-Danforth</t>
+  </si>
+  <si>
+    <t>Edenbridge-Humber Valley</t>
+  </si>
+  <si>
+    <t>Eglinton East</t>
+  </si>
+  <si>
+    <t>Elms-Old Rexdale</t>
+  </si>
+  <si>
+    <t>Englemount-Lawrence</t>
+  </si>
+  <si>
+    <t>Eringate-Centennial-West Deane</t>
+  </si>
+  <si>
+    <t>Etobicoke West Mall</t>
+  </si>
+  <si>
+    <t>Flemingdon Park</t>
+  </si>
+  <si>
+    <t>Forest Hill North</t>
+  </si>
+  <si>
+    <t>Forest Hill South</t>
+  </si>
+  <si>
+    <t>Glenfield-Jane Heights</t>
+  </si>
+  <si>
+    <t>Greenwood-Coxwell</t>
+  </si>
+  <si>
+    <t>Guildwood</t>
+  </si>
+  <si>
+    <t>Henry Farm</t>
+  </si>
+  <si>
+    <t>High Park North</t>
+  </si>
+  <si>
+    <t>High Park-Swansea</t>
+  </si>
+  <si>
+    <t>Highland Creek</t>
+  </si>
+  <si>
+    <t>Hillcrest Village</t>
+  </si>
+  <si>
+    <t>Humber Heights-Westmount</t>
+  </si>
+  <si>
+    <t>Humber Summit</t>
+  </si>
+  <si>
+    <t>Humbermede</t>
+  </si>
+  <si>
+    <t>Humewood-Cedarvale</t>
+  </si>
+  <si>
+    <t>Ionview</t>
+  </si>
+  <si>
+    <t>Islington-City Centre West</t>
+  </si>
+  <si>
+    <t>Junction Area</t>
+  </si>
+  <si>
+    <t>Keelesdale-Eglinton West</t>
+  </si>
+  <si>
+    <t>Kennedy Park</t>
+  </si>
+  <si>
+    <t>Kensington-Chinatown</t>
+  </si>
+  <si>
+    <t>Kingsview Village-The Westway</t>
+  </si>
+  <si>
+    <t>Kingsway South</t>
+  </si>
+  <si>
+    <t>Lambton Baby Point</t>
+  </si>
+  <si>
+    <t>L'Amoreaux</t>
+  </si>
+  <si>
+    <t>Lansing-Westgate</t>
+  </si>
+  <si>
+    <t>Lawrence Park North</t>
+  </si>
+  <si>
+    <t>Lawrence Park South</t>
+  </si>
+  <si>
+    <t>Leaside-Bennington</t>
+  </si>
+  <si>
+    <t>Little Portugal</t>
+  </si>
+  <si>
+    <t>Long Branch</t>
+  </si>
+  <si>
+    <t>Malvern</t>
+  </si>
+  <si>
+    <t>Maple Leaf</t>
+  </si>
+  <si>
+    <t>Markland Wood</t>
+  </si>
+  <si>
+    <t>Milliken</t>
+  </si>
+  <si>
+    <t>Mimico (includes Humber Bay Shores)</t>
+  </si>
+  <si>
+    <t>Morningside</t>
+  </si>
+  <si>
+    <t>Moss Park</t>
+  </si>
+  <si>
+    <t>Mount Dennis</t>
+  </si>
+  <si>
+    <t>Mount Olive-Silverstone-Jamestown</t>
+  </si>
+  <si>
+    <t>Mount Pleasant East</t>
+  </si>
+  <si>
+    <t>Mount Pleasant West</t>
+  </si>
+  <si>
+    <t>New Toronto</t>
+  </si>
+  <si>
+    <t>Newtonbrook East</t>
+  </si>
+  <si>
+    <t>Newtonbrook West</t>
+  </si>
+  <si>
+    <t>Niagara</t>
+  </si>
+  <si>
+    <t>North Riverdale</t>
+  </si>
+  <si>
+    <t>North St. James Town</t>
+  </si>
+  <si>
+    <t>Oakridge</t>
+  </si>
+  <si>
+    <t>Oakwood Village</t>
+  </si>
+  <si>
+    <t>O'Connor-Parkview</t>
+  </si>
+  <si>
+    <t>Old East York</t>
+  </si>
+  <si>
+    <t>Palmerston-Little Italy</t>
+  </si>
+  <si>
+    <t>Parkwoods-Donalda</t>
+  </si>
+  <si>
+    <t>Pelmo Park-Humberlea</t>
+  </si>
+  <si>
+    <t>Playter Estates-Danforth</t>
+  </si>
+  <si>
+    <t>Pleasant View</t>
+  </si>
+  <si>
+    <t>Princess-Rosethorn</t>
+  </si>
+  <si>
+    <t>Regent Park</t>
+  </si>
+  <si>
+    <t>Rexdale-Kipling</t>
+  </si>
+  <si>
+    <t>Rockcliffe-Smythe</t>
+  </si>
+  <si>
+    <t>Roncesvalles</t>
+  </si>
+  <si>
+    <t>Rosedale-Moore Park</t>
+  </si>
+  <si>
+    <t>Rouge</t>
+  </si>
+  <si>
+    <t>Runnymede-Bloor West Village</t>
+  </si>
+  <si>
+    <t>Rustic</t>
+  </si>
+  <si>
+    <t>Scarborough Village</t>
+  </si>
+  <si>
+    <t>South Parkdale</t>
+  </si>
+  <si>
+    <t>South Riverdale</t>
+  </si>
+  <si>
+    <t>St.Andrew-Windfields</t>
+  </si>
+  <si>
+    <t>Steeles</t>
+  </si>
+  <si>
+    <t>Stonegate-Queensway</t>
+  </si>
+  <si>
+    <t>Tam O'Shanter-Sullivan</t>
+  </si>
+  <si>
+    <t>Taylor-Massey</t>
+  </si>
+  <si>
+    <t>The Beaches</t>
+  </si>
+  <si>
+    <t>Thistletown-Beaumond Heights</t>
+  </si>
+  <si>
+    <t>Thorncliffe Park</t>
+  </si>
+  <si>
+    <t>Trinity-Bellwoods</t>
+  </si>
+  <si>
+    <t>University</t>
+  </si>
+  <si>
+    <t>Victoria Village</t>
+  </si>
+  <si>
+    <t>Waterfront Communities-The Island</t>
+  </si>
+  <si>
+    <t>West Hill</t>
+  </si>
+  <si>
+    <t>West Humber-Clairville</t>
+  </si>
+  <si>
+    <t>Westminster-Branson</t>
+  </si>
+  <si>
+    <t>Weston</t>
+  </si>
+  <si>
+    <t>Weston-Pelham Park</t>
+  </si>
+  <si>
+    <t>Wexford/Maryvale</t>
+  </si>
+  <si>
+    <t>Willowdale East</t>
+  </si>
+  <si>
+    <t>Willowdale West</t>
+  </si>
+  <si>
+    <t>Willowridge-Martingrove-Richview</t>
+  </si>
+  <si>
+    <t>Woburn</t>
+  </si>
+  <si>
+    <t>Woodbine Corridor</t>
+  </si>
+  <si>
+    <t>Woodbine-Lumsden</t>
+  </si>
+  <si>
+    <t>Wychwood</t>
+  </si>
+  <si>
+    <t>Yonge-Eglinton</t>
+  </si>
+  <si>
+    <t>Yonge-St.Clair</t>
+  </si>
+  <si>
+    <t>York University Heights</t>
+  </si>
+  <si>
+    <t>Yorkdale-Glen Park</t>
   </si>
 </sst>
 </file>
@@ -472,10 +910,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D8BC7F4-40D3-8143-BDD2-269D7F8A7853}">
-  <dimension ref="A2:EP26"/>
+  <dimension ref="A1:EP26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -484,6 +922,446 @@
     <col min="5" max="5" width="77.5" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:146" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R1" t="s">
+        <v>46</v>
+      </c>
+      <c r="S1" t="s">
+        <v>47</v>
+      </c>
+      <c r="T1" t="s">
+        <v>48</v>
+      </c>
+      <c r="U1" t="s">
+        <v>49</v>
+      </c>
+      <c r="V1" t="s">
+        <v>50</v>
+      </c>
+      <c r="W1" t="s">
+        <v>51</v>
+      </c>
+      <c r="X1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>81</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>82</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>86</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>87</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>89</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>90</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>92</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>94</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>95</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>96</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>97</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>100</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>101</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>102</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>103</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>104</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>105</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>106</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>107</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>108</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>109</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>110</v>
+      </c>
+      <c r="CE1" t="s">
+        <v>111</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>112</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>113</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>114</v>
+      </c>
+      <c r="CI1" t="s">
+        <v>115</v>
+      </c>
+      <c r="CJ1" t="s">
+        <v>116</v>
+      </c>
+      <c r="CK1" t="s">
+        <v>117</v>
+      </c>
+      <c r="CL1" t="s">
+        <v>118</v>
+      </c>
+      <c r="CM1" t="s">
+        <v>119</v>
+      </c>
+      <c r="CN1" t="s">
+        <v>120</v>
+      </c>
+      <c r="CO1" t="s">
+        <v>121</v>
+      </c>
+      <c r="CP1" t="s">
+        <v>122</v>
+      </c>
+      <c r="CQ1" t="s">
+        <v>123</v>
+      </c>
+      <c r="CR1" t="s">
+        <v>124</v>
+      </c>
+      <c r="CS1" t="s">
+        <v>125</v>
+      </c>
+      <c r="CT1" t="s">
+        <v>126</v>
+      </c>
+      <c r="CU1" t="s">
+        <v>127</v>
+      </c>
+      <c r="CV1" t="s">
+        <v>128</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>129</v>
+      </c>
+      <c r="CX1" t="s">
+        <v>130</v>
+      </c>
+      <c r="CY1" t="s">
+        <v>131</v>
+      </c>
+      <c r="CZ1" t="s">
+        <v>132</v>
+      </c>
+      <c r="DA1" t="s">
+        <v>133</v>
+      </c>
+      <c r="DB1" t="s">
+        <v>134</v>
+      </c>
+      <c r="DC1" t="s">
+        <v>135</v>
+      </c>
+      <c r="DD1" t="s">
+        <v>136</v>
+      </c>
+      <c r="DE1" t="s">
+        <v>137</v>
+      </c>
+      <c r="DF1" t="s">
+        <v>138</v>
+      </c>
+      <c r="DG1" t="s">
+        <v>139</v>
+      </c>
+      <c r="DH1" t="s">
+        <v>140</v>
+      </c>
+      <c r="DI1" t="s">
+        <v>141</v>
+      </c>
+      <c r="DJ1" t="s">
+        <v>142</v>
+      </c>
+      <c r="DK1" t="s">
+        <v>143</v>
+      </c>
+      <c r="DL1" t="s">
+        <v>144</v>
+      </c>
+      <c r="DM1" t="s">
+        <v>145</v>
+      </c>
+      <c r="DN1" t="s">
+        <v>146</v>
+      </c>
+      <c r="DO1" t="s">
+        <v>147</v>
+      </c>
+      <c r="DP1" t="s">
+        <v>148</v>
+      </c>
+      <c r="DQ1" t="s">
+        <v>149</v>
+      </c>
+      <c r="DR1" t="s">
+        <v>150</v>
+      </c>
+      <c r="DS1" t="s">
+        <v>151</v>
+      </c>
+      <c r="DT1" t="s">
+        <v>152</v>
+      </c>
+      <c r="DU1" t="s">
+        <v>153</v>
+      </c>
+      <c r="DV1" t="s">
+        <v>154</v>
+      </c>
+      <c r="DW1" t="s">
+        <v>155</v>
+      </c>
+      <c r="DX1" t="s">
+        <v>156</v>
+      </c>
+      <c r="DY1" t="s">
+        <v>157</v>
+      </c>
+      <c r="DZ1" t="s">
+        <v>158</v>
+      </c>
+      <c r="EA1" t="s">
+        <v>159</v>
+      </c>
+      <c r="EB1" t="s">
+        <v>160</v>
+      </c>
+      <c r="EC1" t="s">
+        <v>161</v>
+      </c>
+      <c r="ED1" t="s">
+        <v>162</v>
+      </c>
+      <c r="EE1" t="s">
+        <v>163</v>
+      </c>
+      <c r="EF1" t="s">
+        <v>164</v>
+      </c>
+      <c r="EG1" t="s">
+        <v>165</v>
+      </c>
+      <c r="EH1" t="s">
+        <v>166</v>
+      </c>
+      <c r="EI1" t="s">
+        <v>167</v>
+      </c>
+      <c r="EJ1" t="s">
+        <v>168</v>
+      </c>
+      <c r="EK1" t="s">
+        <v>169</v>
+      </c>
+      <c r="EL1" t="s">
+        <v>170</v>
+      </c>
+      <c r="EM1" t="s">
+        <v>171</v>
+      </c>
+      <c r="EN1" t="s">
+        <v>172</v>
+      </c>
+      <c r="EO1" t="s">
+        <v>173</v>
+      </c>
+      <c r="EP1" t="s">
+        <v>174</v>
+      </c>
+    </row>
     <row r="2" spans="1:146" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>27</v>

</xml_diff>